<commit_message>
4_1_text_to_code refined and workiing
</commit_message>
<xml_diff>
--- a/TextData/Prompts_TestData.xlsx
+++ b/TextData/Prompts_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d535f39b5ea74528/2020_Y1/PhD/Y_Conferences^MPaper/17_CAADRIA2025/HRI_LLM/TextData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_08D552B3D37056396F9A2911595ED87656CDFB87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{483BD2B2-BD16-4F23-817D-07C554B238F1}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_55C933ABD3C05731B7B83511595ED87656CDDB89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FA8EB34-00B7-472A-BA53-00F70097CCD0}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -694,14 +694,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+      <selection activeCell="C2" sqref="C2:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="61.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>